<commit_message>
Added TableColumnModel + Constants
</commit_message>
<xml_diff>
--- a/src/PropertyManager/PropertyManager/PropertyManager/Resources/Data.xlsx
+++ b/src/PropertyManager/PropertyManager/PropertyManager/Resources/Data.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simonj\Desktop\sdfsd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\xplat-graph\src\PropertyManager\PropertyManager\PropertyManager\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12015"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Charts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -130,8 +131,8 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Book1.xlsx]Sheet1!PivotTable2</c:name>
-    <c:fmtId val="0"/>
+    <c:name>[Data.xlsx]Charts!PivotTable2</c:name>
+    <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
@@ -181,20 +182,37 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="diamond"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -209,7 +227,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$5</c:f>
+              <c:f>Charts!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -233,7 +251,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$K$6:$K$7</c:f>
+              <c:f>Charts!$D$3:$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -244,7 +262,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$6:$L$7</c:f>
+              <c:f>Charts!$E$3:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -253,7 +271,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-96CB-450D-A876-527271F0DC97}"/>
+              <c16:uniqueId val="{00000000-70D0-4D45-BED9-E02A2D268BE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1011,21 +1029,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1045,7 +1065,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Simon Jäger" refreshedDate="42541.772496412035" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="2">
   <cacheSource type="worksheet">
-    <worksheetSource name="Table1"/>
+    <worksheetSource name="PropertyTable"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="ID" numFmtId="0">
@@ -1101,8 +1121,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="K5:L7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="D2:E4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -1135,8 +1155,17 @@
   <dataFields count="1">
     <dataField name="Sum of OperatingCosts" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="3" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1156,8 +1185,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F3" totalsRowShown="0">
-  <autoFilter ref="A1:F3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PropertyTable" displayName="PropertyTable" ref="A1:F2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:F2"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Description"/>
@@ -1467,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,7 +1512,7 @@
     <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1503,31 +1532,46 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K5" s="2" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L5" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K6" s="3" t="s">
+    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="E3" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K7" s="3" t="s">
+    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Services + Models
</commit_message>
<xml_diff>
--- a/src/PropertyManager/PropertyManager/PropertyManager/Resources/Data.xlsx
+++ b/src/PropertyManager/PropertyManager/PropertyManager/Resources/Data.xlsx
@@ -30,9 +30,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>(blank)</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1188,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PropertyTable" displayName="PropertyTable" ref="A1:F2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:F2"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID"/>
+    <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Rooms"/>
     <tableColumn id="4" name="LivingArea"/>
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,22 +1514,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1552,21 +1552,21 @@
   <sheetData>
     <row r="2" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1"/>
     </row>

</xml_diff>

<commit_message>
Fixed Group Drive Creation Bug
</commit_message>
<xml_diff>
--- a/src/PropertyManager/PropertyManager/PropertyManager/Resources/Data.xlsx
+++ b/src/PropertyManager/PropertyManager/PropertyManager/Resources/Data.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\xplat-graph\src\PropertyManager\PropertyManager\PropertyManager\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="20" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,9 +45,6 @@
     <t>OperatingCosts</t>
   </si>
   <si>
-    <t>Sum of OperatingCosts</t>
-  </si>
-  <si>
     <t>Row Labels</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>Sum of LivingArea</t>
   </si>
 </sst>
 </file>
@@ -131,47 +131,41 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Data.xlsx]Charts!PivotTable2</c:name>
-    <c:fmtId val="2"/>
+    <c:name>[Data.xlsx]Charts!PivotTable1</c:name>
+    <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -180,13 +174,62 @@
             <a:noFill/>
           </a:ln>
           <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="50800" h="101600" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
         </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="2"/>
+        <c:idx val="13"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -195,13 +238,20 @@
             <a:noFill/>
           </a:ln>
           <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="0" h="0" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
         </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="3"/>
+        <c:idx val="14"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -210,24 +260,73 @@
             <a:noFill/>
           </a:ln>
           <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="0" h="0" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
         </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="0" h="0" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="0" h="0" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$E$2</c:f>
+              <c:f>Charts!$F$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -237,21 +336,93 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-F0BF-49ED-91AF-E9E4DA65E65A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
-            <c:delete val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Charts!$D$3:$D$4</c:f>
+              <c:f>Charts!$E$8:$E$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -262,7 +433,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$E$3:$E$4</c:f>
+              <c:f>Charts!$F$8:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -271,104 +442,22 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-70D0-4D45-BED9-E02A2D268BE0}"/>
+              <c16:uniqueId val="{00000004-F0BF-49ED-91AF-E9E4DA65E65A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
-          <c:showCatName val="0"/>
+          <c:showCatName val="1"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:gapWidth val="444"/>
-        <c:overlap val="-90"/>
-        <c:axId val="353438512"/>
-        <c:axId val="353431952"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="353438512"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="353431952"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="353431952"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353438512"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="43"/>
+      </c:doughnutChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -377,44 +466,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -446,7 +504,6 @@
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
         <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
@@ -502,7 +559,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -513,7 +570,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -525,7 +582,19 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -536,29 +605,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
@@ -566,15 +612,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
-    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -611,12 +651,22 @@
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="brightRoom" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat">
+        <a:bevelT w="50800" h="101600" prst="angle"/>
+        <a:contourClr>
+          <a:srgbClr val="000000"/>
+        </a:contourClr>
+      </a:sp3d>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -626,12 +676,17 @@
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -641,10 +696,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -653,15 +708,13 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -669,13 +722,12 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -683,7 +735,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -705,13 +757,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -721,7 +775,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -730,135 +784,205 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -868,77 +992,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -947,7 +1001,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -968,26 +1022,27 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1001,17 +1056,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1019,8 +1063,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1029,23 +1079,21 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1063,16 +1111,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Simon Jäger" refreshedDate="42541.772496412035" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="2">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Simon Jäger" refreshedDate="42560.043461458336" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="PropertyTable"/>
   </cacheSource>
   <cacheFields count="6">
-    <cacheField name="ID" numFmtId="0">
-      <sharedItems containsNonDate="0" containsBlank="1" count="3">
+    <cacheField name="Id" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="5">
         <m/>
-        <s v="Test" u="1"/>
-        <s v="Test 2" u="1"/>
+        <n v="2" u="1"/>
+        <n v="1" u="1"/>
+        <n v="3" u="1"/>
+        <n v="4" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Description" numFmtId="0">
@@ -1100,15 +1150,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="2">
-  <r>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
   <r>
     <x v="0"/>
     <m/>
@@ -1121,29 +1163,31 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="D2:E4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="E7:F9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
-      <items count="4">
+      <items count="6">
+        <item m="1" x="2"/>
         <item m="1" x="1"/>
-        <item m="1" x="2"/>
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
   <rowItems count="2">
     <i>
-      <x v="2"/>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -1153,10 +1197,10 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of OperatingCosts" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of LivingArea" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="1" series="1">
+  <chartFormats count="5">
+    <chartFormat chart="0" format="12" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1165,11 +1209,50 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="3" series="1">
+    <chartFormat chart="0" format="13">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -1202,7 +1285,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Red Violet">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1210,34 +1293,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="454551"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="D8D9DC"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="E32D91"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C830CC"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="4EA6DC"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="4775E7"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="8971E1"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="D54773"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="6B9F25"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="8C8C8C"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -1498,23 +1581,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="9.375" customWidth="1"/>
+    <col min="6" max="6" width="16.75" customWidth="1"/>
+    <col min="11" max="11" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1542,33 +1625,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:E4"/>
+  <dimension ref="D3:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="7" max="9" width="1.875" customWidth="1"/>
+    <col min="10" max="10" width="9.875" customWidth="1"/>
+    <col min="11" max="11" width="4.5" customWidth="1"/>
+    <col min="12" max="12" width="7.25" customWidth="1"/>
+    <col min="13" max="13" width="9.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D2" s="2" t="s">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1"/>
+      <c r="F9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Task Add + Complete
</commit_message>
<xml_diff>
--- a/src/PropertyManager/PropertyManager/PropertyManager/Resources/Data.xlsx
+++ b/src/PropertyManager/PropertyManager/PropertyManager/Resources/Data.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -150,7 +150,7 @@
         <c:idx val="3"/>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="11"/>
+        <c:idx val="4"/>
         <c:dLbl>
           <c:idx val="0"/>
           <c:showLegendKey val="0"/>
@@ -165,7 +165,7 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="12"/>
+        <c:idx val="5"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -186,8 +186,7 @@
           </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -229,7 +228,7 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="13"/>
+        <c:idx val="6"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -251,7 +250,7 @@
         </c:spPr>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="14"/>
+        <c:idx val="7"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -273,7 +272,7 @@
         </c:spPr>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="15"/>
+        <c:idx val="8"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -295,7 +294,7 @@
         </c:spPr>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="16"/>
+        <c:idx val="9"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -316,6 +315,53 @@
           </a:sp3d>
         </c:spPr>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="50800" h="101600" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="50800" h="101600" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -335,11 +381,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -369,56 +410,7 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1079,16 +1071,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>185739</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1163,7 +1155,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="E7:F9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -1199,60 +1191,12 @@
   <dataFields count="1">
     <dataField name="Sum of LivingArea" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="12" series="1">
+  <chartFormats count="1">
+    <chartFormat chart="0" format="11" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="16">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -1582,7 +1526,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,18 +1572,14 @@
   <dimension ref="D3:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="14.875" customWidth="1"/>
-    <col min="7" max="9" width="1.875" customWidth="1"/>
-    <col min="10" max="10" width="9.875" customWidth="1"/>
-    <col min="11" max="11" width="4.5" customWidth="1"/>
-    <col min="12" max="12" width="7.25" customWidth="1"/>
-    <col min="13" max="13" width="9.875" customWidth="1"/>
+    <col min="7" max="8" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>